<commit_message>
Most recent results with new scree plot
</commit_message>
<xml_diff>
--- a/data/processed/Overview_of_results.xlsx
+++ b/data/processed/Overview_of_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizmedeiros/Documents/covid/covid-drivers/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BF29B8-7EB2-FE43-867F-1182FA8AE78A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0ED074-F030-DA49-AA3E-84FB68C21FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1480" yWindow="-24000" windowWidth="38400" windowHeight="24000" xr2:uid="{7CA77637-F8F5-8C43-91E2-0857DED38949}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{7CA77637-F8F5-8C43-91E2-0857DED38949}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>Method</t>
   </si>
@@ -192,6 +192,55 @@
   </si>
   <si>
     <t xml:space="preserve">With all components and for test where independent Hops variable is added (without PCA) and removed, p-value is 0.005038295 and estimate for Hosp variable is 1.548151e-05. In other words, difference in hospital beds has a positive correlation with difference in deaths and has a statistically significant effect on the model. For keeping only 12 components (90% variance, p-value is 3.900125e-05 with estimate for Hospital bed variable being 2.405666e-05. For keeping only 8 components (81% variance), p-value is  7.347416e-05 with estimate being 2.559641e-05. </t>
+  </si>
+  <si>
+    <t>same as above but with capping both hospital beds and nursing homes each at 75th percentile. Also redid scree plot with variances of successive PCs instead of toal variance and found inflection point at 5 components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scree plot was done incorrectly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Likelihood -ratio tests on PCA data with Hospital Beds with capped number of Hospital beds and Nursing Homes (both capped at 75th percentile at county level) and with land Area                                                                                                 </t>
+  </si>
+  <si>
+    <t>Variables list: 
+Independent variables 
+1 Month Prior Intra-Mobility
+1 Month Prior Inter-Mobility
+2wk Prior Intra-Mobility
+2wk Onset Intra-Mobility
+2wk Post Intra-Mobility
+2wk Prior Inter-Mobility
+2wk Onset Inter-Mobility
+2wk Post Inter-Mobility
+[all mobility is as number of trips normalized by population]
+Density per square mile of land area - Population
+Rural-urban_Continuum Code_2013
+Percent of adults with less than a high school diploma 2014-18
+Percent of adults with a bachelor's degree or higher 2014-18
+Unemployment_rate_2018
+Med_HH_Income_Percent_of_State_Total_2018
+Total_age65plus normalized by population 
+Total households!!Average household size
+SCHOOL ENROLLMENT!!Population 3 years and over enrolled in school!!Nursery school preschool
+SCHOOL ENROLLMENT!!Population 3 years and over enrolled in school!!Kindergarten
+SCHOOL ENROLLMENT!!Population 3 years and over enrolled in school!!Elementary school (grades 1-8)
+SCHOOL ENROLLMENT!!Population 3 years and over enrolled in school!!High school (grades 9-12)
+SCHOOL ENROLLMENT!!Population 3 years and over enrolled in school!!College or graduate school
+[all school enrollment variables are normalized by pop] 
+Area in square miles - Land area
+NursingCt- number of nursing homes normalized by county population 
+HospCt - number of hospital beds per county normalized by county population 
+Hispanic Population- fraction of pop
+Black Population- fraction of pop 
+Outbreak Month Temp AVG / F
+Time from outbreak to intervention
+Time from outbreak to national intervention
+Time from national intervention to outbreak
+Dependent variable: deaths normalized by pop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With 5 components kept and for test where independent Hops variable is added (without PCA) and removed, p-value is 0.003820024 and estimate for Hosp variable is 2.945047e-05. The test statistic for the likelihoosd ratio test was F=8.367445. </t>
   </si>
 </sst>
 </file>
@@ -583,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B819FE97-8A8C-0747-9347-2A3D2C3420B4}">
   <dimension ref="A2:O88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -593,6 +642,7 @@
     <col min="3" max="3" width="64" customWidth="1"/>
     <col min="4" max="4" width="39.83203125" customWidth="1"/>
     <col min="5" max="5" width="60.5" customWidth="1"/>
+    <col min="6" max="6" width="124.6640625" customWidth="1"/>
     <col min="9" max="9" width="67.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -834,15 +884,28 @@
       <c r="D14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+    <row r="15" spans="1:15" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
@@ -874,7 +937,6 @@
       <c r="C19" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>

</xml_diff>